<commit_message>
Updated DEU_grids model - 2025-09-04 12:49
</commit_message>
<xml_diff>
--- a/VerveStacks_DEU_grids/SuppXLS/scen_tsparameters_ts12_clu.xlsx
+++ b/VerveStacks_DEU_grids/SuppXLS/scen_tsparameters_ts12_clu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_DEU_grids\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{555195EB-9D5D-4D4C-86A5-23422B46E42B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{503C751F-9B0E-44ED-B84A-8D66868D4B9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="1" activeTab="1" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -1902,13 +1902,13 @@
     <t>D</t>
   </si>
   <si>
-    <t>S2aH2,S1aH3,S1aH2,S2aH3,S3aH3,S3aH2</t>
+    <t>S3aH2,S2aH2,S1aH2,S2aH3,S3aH3,S1aH3</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>S3aH1,S2aH4,S1aH4,S2aH1,S1aH1,S3aH4</t>
+    <t>S1aH1,S3aH4,S1aH4,S2aH1,S2aH4,S3aH1</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -2511,7 +2511,7 @@
       </c>
       <c r="H23" t="str">
         <f>HLOOKUP($A$10,$D$10:$CU$12,3,FALSE)</f>
-        <v>S3aH1,S2aH4,S1aH4,S2aH1,S1aH1,S3aH4</v>
+        <v>S1aH1,S3aH4,S1aH4,S2aH1,S2aH4,S3aH1</v>
       </c>
       <c r="I23">
         <f>1+I24</f>
@@ -2543,7 +2543,7 @@
       </c>
       <c r="H24" t="str">
         <f>HLOOKUP($A$10,$D$10:$CU$12,2,FALSE)</f>
-        <v>S2aH2,S1aH3,S1aH2,S2aH3,S3aH3,S3aH2</v>
+        <v>S3aH2,S2aH2,S1aH2,S2aH3,S3aH3,S1aH3</v>
       </c>
       <c r="I24">
         <f>-$I$17</f>
@@ -2559,7 +2559,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E476185F-FC98-4B6C-B102-346FFB28AB12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8ADE49B-EB16-4895-BD26-C9E3CF8E8970}">
   <dimension ref="A9:AM2278"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -2785,7 +2785,7 @@
         <v>22</v>
       </c>
       <c r="AL11">
-        <v>1.0411103488310731</v>
+        <v>1.0411103488310727</v>
       </c>
       <c r="AM11" t="s">
         <v>628</v>
@@ -2871,7 +2871,7 @@
         <v>28</v>
       </c>
       <c r="AL12">
-        <v>8.4099424771755776E-2</v>
+        <v>8.4099424771755762E-2</v>
       </c>
       <c r="AM12" t="s">
         <v>628</v>
@@ -2957,7 +2957,7 @@
         <v>26</v>
       </c>
       <c r="AL13">
-        <v>7.4790226397171367E-2</v>
+        <v>7.4790226397171353E-2</v>
       </c>
       <c r="AM13" t="s">
         <v>628</v>

</xml_diff>